<commit_message>
Auto push 2023-03-20 10:03:01.67
</commit_message>
<xml_diff>
--- a/project/shin_movie.xlsx
+++ b/project/shin_movie.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="192">
   <si>
     <t>이용자 권한과 기능</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -737,10 +737,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>searchResult.jsp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>userId, userPw</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -750,6 +746,38 @@
   </si>
   <si>
     <t>boardId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영화 등록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영화 수정(개봉예정,상영작,종료)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>인물 등록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>인물 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원 제재</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>검색 결과페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>searchResult.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>searchResult.do</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1245,7 +1273,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1435,12 +1463,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1450,42 +1517,39 @@
     <xf numFmtId="0" fontId="4" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1504,35 +1568,8 @@
     <xf numFmtId="0" fontId="11" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1900,41 +1937,41 @@
     <row r="1" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="66" t="s">
         <v>134</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73"/>
-      <c r="N2" s="73"/>
-      <c r="O2" s="73"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="67"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="67"/>
+      <c r="O2" s="67"/>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
-      <c r="B3" s="73"/>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
-      <c r="K3" s="73"/>
-      <c r="L3" s="73"/>
-      <c r="M3" s="73"/>
-      <c r="N3" s="73"/>
-      <c r="O3" s="73"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
+      <c r="L3" s="67"/>
+      <c r="M3" s="67"/>
+      <c r="N3" s="67"/>
+      <c r="O3" s="67"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
     </row>
@@ -1979,32 +2016,32 @@
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="20"/>
-      <c r="C6" s="74" t="s">
+      <c r="C6" s="68" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="39"/>
-      <c r="E6" s="76" t="s">
+      <c r="E6" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="76"/>
-      <c r="G6" s="76"/>
-      <c r="H6" s="76"/>
-      <c r="I6" s="76"/>
-      <c r="J6" s="76"/>
-      <c r="K6" s="77"/>
-      <c r="L6" s="78" t="s">
+      <c r="F6" s="70"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="70"/>
+      <c r="J6" s="70"/>
+      <c r="K6" s="71"/>
+      <c r="L6" s="72" t="s">
         <v>35</v>
       </c>
-      <c r="M6" s="76"/>
-      <c r="N6" s="76"/>
-      <c r="O6" s="76"/>
+      <c r="M6" s="70"/>
+      <c r="N6" s="70"/>
+      <c r="O6" s="70"/>
       <c r="P6" s="21"/>
       <c r="Q6" s="5"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
       <c r="B7" s="13"/>
-      <c r="C7" s="75"/>
+      <c r="C7" s="69"/>
       <c r="D7" s="22"/>
       <c r="E7" s="13">
         <v>20</v>
@@ -2104,7 +2141,7 @@
     <row r="11" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="6"/>
-      <c r="C11" s="68" t="s">
+      <c r="C11" s="73" t="s">
         <v>33</v>
       </c>
       <c r="D11" s="10"/>
@@ -2125,7 +2162,7 @@
     <row r="12" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="68"/>
+      <c r="C12" s="73"/>
       <c r="D12" s="10"/>
       <c r="E12" s="8"/>
       <c r="F12" s="6"/>
@@ -2163,7 +2200,7 @@
     <row r="14" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="6"/>
-      <c r="C14" s="71" t="s">
+      <c r="C14" s="65" t="s">
         <v>34</v>
       </c>
       <c r="D14" s="10"/>
@@ -2184,7 +2221,7 @@
     <row r="15" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="71"/>
+      <c r="C15" s="65"/>
       <c r="D15" s="10"/>
       <c r="E15" s="8"/>
       <c r="F15" s="6"/>
@@ -2222,7 +2259,7 @@
     <row r="17" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16"/>
       <c r="B17" s="6"/>
-      <c r="C17" s="68" t="s">
+      <c r="C17" s="73" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="10"/>
@@ -2243,7 +2280,7 @@
     <row r="18" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="16"/>
       <c r="B18" s="6"/>
-      <c r="C18" s="68"/>
+      <c r="C18" s="73"/>
       <c r="D18" s="10"/>
       <c r="E18" s="6"/>
       <c r="F18" s="8"/>
@@ -2302,7 +2339,7 @@
     <row r="21" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="16"/>
       <c r="B21" s="6"/>
-      <c r="C21" s="69" t="s">
+      <c r="C21" s="75" t="s">
         <v>12</v>
       </c>
       <c r="D21" s="10"/>
@@ -2323,7 +2360,7 @@
     <row r="22" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="16"/>
       <c r="B22" s="6"/>
-      <c r="C22" s="69"/>
+      <c r="C22" s="75"/>
       <c r="D22" s="10"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
@@ -2361,7 +2398,7 @@
     <row r="24" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="16"/>
       <c r="B24" s="6"/>
-      <c r="C24" s="69" t="s">
+      <c r="C24" s="75" t="s">
         <v>16</v>
       </c>
       <c r="D24" s="10"/>
@@ -2382,7 +2419,7 @@
     <row r="25" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="16"/>
       <c r="B25" s="6"/>
-      <c r="C25" s="69"/>
+      <c r="C25" s="75"/>
       <c r="D25" s="10"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
@@ -2420,7 +2457,7 @@
     <row r="27" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="16"/>
       <c r="B27" s="6"/>
-      <c r="C27" s="69" t="s">
+      <c r="C27" s="75" t="s">
         <v>135</v>
       </c>
       <c r="D27" s="10"/>
@@ -2441,7 +2478,7 @@
     <row r="28" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="16"/>
       <c r="B28" s="6"/>
-      <c r="C28" s="69"/>
+      <c r="C28" s="75"/>
       <c r="D28" s="10"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
@@ -2479,7 +2516,7 @@
     <row r="30" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="16"/>
       <c r="B30" s="6"/>
-      <c r="C30" s="69" t="s">
+      <c r="C30" s="75" t="s">
         <v>136</v>
       </c>
       <c r="D30" s="10"/>
@@ -2500,7 +2537,7 @@
     <row r="31" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="16"/>
       <c r="B31" s="6"/>
-      <c r="C31" s="69"/>
+      <c r="C31" s="75"/>
       <c r="D31" s="10"/>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
@@ -2538,7 +2575,7 @@
     <row r="33" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="16"/>
       <c r="B33" s="6"/>
-      <c r="C33" s="69" t="s">
+      <c r="C33" s="75" t="s">
         <v>137</v>
       </c>
       <c r="D33" s="10"/>
@@ -2559,7 +2596,7 @@
     <row r="34" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="16"/>
       <c r="B34" s="6"/>
-      <c r="C34" s="69"/>
+      <c r="C34" s="75"/>
       <c r="D34" s="10"/>
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
@@ -2637,7 +2674,7 @@
     <row r="38" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="16"/>
       <c r="B38" s="6"/>
-      <c r="C38" s="70" t="s">
+      <c r="C38" s="76" t="s">
         <v>15</v>
       </c>
       <c r="D38" s="10"/>
@@ -2658,7 +2695,7 @@
     <row r="39" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="16"/>
       <c r="B39" s="6"/>
-      <c r="C39" s="70"/>
+      <c r="C39" s="76"/>
       <c r="D39" s="10"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
@@ -2696,7 +2733,7 @@
     <row r="41" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="16"/>
       <c r="B41" s="6"/>
-      <c r="C41" s="70" t="s">
+      <c r="C41" s="76" t="s">
         <v>14</v>
       </c>
       <c r="D41" s="10"/>
@@ -2717,7 +2754,7 @@
     <row r="42" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="16"/>
       <c r="B42" s="6"/>
-      <c r="C42" s="70"/>
+      <c r="C42" s="76"/>
       <c r="D42" s="10"/>
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
@@ -2755,7 +2792,7 @@
     <row r="44" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="16"/>
       <c r="B44" s="6"/>
-      <c r="C44" s="70" t="s">
+      <c r="C44" s="76" t="s">
         <v>161</v>
       </c>
       <c r="D44" s="10"/>
@@ -2776,7 +2813,7 @@
     <row r="45" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="16"/>
       <c r="B45" s="6"/>
-      <c r="C45" s="70"/>
+      <c r="C45" s="76"/>
       <c r="D45" s="10"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
@@ -2814,7 +2851,7 @@
     <row r="47" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="16"/>
       <c r="B47" s="6"/>
-      <c r="C47" s="70" t="s">
+      <c r="C47" s="76" t="s">
         <v>138</v>
       </c>
       <c r="D47" s="10"/>
@@ -2835,7 +2872,7 @@
     <row r="48" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="16"/>
       <c r="B48" s="6"/>
-      <c r="C48" s="70"/>
+      <c r="C48" s="76"/>
       <c r="D48" s="10"/>
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
@@ -2873,7 +2910,7 @@
     <row r="50" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="16"/>
       <c r="B50" s="6"/>
-      <c r="C50" s="70" t="s">
+      <c r="C50" s="76" t="s">
         <v>162</v>
       </c>
       <c r="D50" s="10"/>
@@ -2894,7 +2931,7 @@
     <row r="51" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="16"/>
       <c r="B51" s="6"/>
-      <c r="C51" s="70"/>
+      <c r="C51" s="76"/>
       <c r="D51" s="10"/>
       <c r="E51" s="6"/>
       <c r="F51" s="6"/>
@@ -2953,7 +2990,7 @@
     <row r="54" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="16"/>
       <c r="B54" s="6"/>
-      <c r="C54" s="64" t="s">
+      <c r="C54" s="74" t="s">
         <v>139</v>
       </c>
       <c r="D54" s="10"/>
@@ -2974,7 +3011,7 @@
     <row r="55" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="16"/>
       <c r="B55" s="6"/>
-      <c r="C55" s="64"/>
+      <c r="C55" s="74"/>
       <c r="D55" s="10"/>
       <c r="E55" s="6"/>
       <c r="F55" s="6"/>
@@ -3012,7 +3049,7 @@
     <row r="57" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="16"/>
       <c r="B57" s="6"/>
-      <c r="C57" s="64" t="s">
+      <c r="C57" s="74" t="s">
         <v>140</v>
       </c>
       <c r="D57" s="10"/>
@@ -3033,7 +3070,7 @@
     <row r="58" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="16"/>
       <c r="B58" s="6"/>
-      <c r="C58" s="64"/>
+      <c r="C58" s="74"/>
       <c r="D58" s="10"/>
       <c r="E58" s="6"/>
       <c r="F58" s="6"/>
@@ -3071,7 +3108,7 @@
     <row r="60" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="16"/>
       <c r="B60" s="6"/>
-      <c r="C60" s="64" t="s">
+      <c r="C60" s="74" t="s">
         <v>160</v>
       </c>
       <c r="D60" s="10"/>
@@ -3092,7 +3129,7 @@
     <row r="61" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="16"/>
       <c r="B61" s="6"/>
-      <c r="C61" s="64"/>
+      <c r="C61" s="74"/>
       <c r="D61" s="10"/>
       <c r="E61" s="6"/>
       <c r="F61" s="6"/>
@@ -3130,7 +3167,7 @@
     <row r="63" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="16"/>
       <c r="B63" s="6"/>
-      <c r="C63" s="64" t="s">
+      <c r="C63" s="74" t="s">
         <v>159</v>
       </c>
       <c r="D63" s="10"/>
@@ -3151,7 +3188,7 @@
     <row r="64" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="16"/>
       <c r="B64" s="6"/>
-      <c r="C64" s="64"/>
+      <c r="C64" s="74"/>
       <c r="D64" s="10"/>
       <c r="E64" s="6"/>
       <c r="F64" s="6"/>
@@ -3189,7 +3226,7 @@
     <row r="66" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="16"/>
       <c r="B66" s="6"/>
-      <c r="C66" s="64" t="s">
+      <c r="C66" s="74" t="s">
         <v>158</v>
       </c>
       <c r="D66" s="10"/>
@@ -3210,7 +3247,7 @@
     <row r="67" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="16"/>
       <c r="B67" s="6"/>
-      <c r="C67" s="64"/>
+      <c r="C67" s="74"/>
       <c r="D67" s="10"/>
       <c r="E67" s="6"/>
       <c r="F67" s="6"/>
@@ -3248,7 +3285,7 @@
     <row r="69" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="16"/>
       <c r="B69" s="6"/>
-      <c r="C69" s="64" t="s">
+      <c r="C69" s="74" t="s">
         <v>157</v>
       </c>
       <c r="D69" s="10"/>
@@ -3269,7 +3306,7 @@
     <row r="70" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="16"/>
       <c r="B70" s="6"/>
-      <c r="C70" s="64"/>
+      <c r="C70" s="74"/>
       <c r="D70" s="10"/>
       <c r="E70" s="6"/>
       <c r="F70" s="6"/>
@@ -3307,7 +3344,7 @@
     <row r="72" spans="1:68" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="16"/>
       <c r="B72" s="6"/>
-      <c r="C72" s="65" t="s">
+      <c r="C72" s="78" t="s">
         <v>57</v>
       </c>
       <c r="D72" s="7"/>
@@ -3328,7 +3365,7 @@
     <row r="73" spans="1:68" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="16"/>
       <c r="B73" s="6"/>
-      <c r="C73" s="65"/>
+      <c r="C73" s="78"/>
       <c r="D73" s="7"/>
       <c r="E73" s="6"/>
       <c r="F73" s="6"/>
@@ -3347,7 +3384,7 @@
     <row r="74" spans="1:68" s="5" customFormat="1" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="16"/>
       <c r="B74" s="6"/>
-      <c r="C74" s="67" t="s">
+      <c r="C74" s="80" t="s">
         <v>133</v>
       </c>
       <c r="D74" s="7"/>
@@ -3418,7 +3455,7 @@
     <row r="75" spans="1:68" s="5" customFormat="1" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="16"/>
       <c r="B75" s="6"/>
-      <c r="C75" s="67"/>
+      <c r="C75" s="80"/>
       <c r="D75" s="7"/>
       <c r="E75" s="6"/>
       <c r="F75" s="6"/>
@@ -3546,18 +3583,18 @@
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
       <c r="E79" s="5"/>
-      <c r="F79" s="66"/>
-      <c r="G79" s="66"/>
+      <c r="F79" s="79"/>
+      <c r="G79" s="79"/>
       <c r="H79" s="6"/>
       <c r="I79" s="38" t="s">
         <v>59</v>
       </c>
       <c r="J79" s="38"/>
       <c r="K79" s="6"/>
-      <c r="L79" s="63" t="s">
+      <c r="L79" s="77" t="s">
         <v>58</v>
       </c>
-      <c r="M79" s="63"/>
+      <c r="M79" s="77"/>
       <c r="N79" s="40"/>
       <c r="O79" s="5"/>
       <c r="P79" s="5"/>
@@ -3583,12 +3620,15 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="B2:O3"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="E6:K6"/>
-    <mergeCell ref="L6:O6"/>
-    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="L79:M79"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="F79:G79"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="C69:C70"/>
     <mergeCell ref="C54:C55"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="C21:C22"/>
@@ -3601,15 +3641,12 @@
     <mergeCell ref="C44:C45"/>
     <mergeCell ref="C50:C51"/>
     <mergeCell ref="C47:C48"/>
-    <mergeCell ref="L79:M79"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="F79:G79"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="C69:C70"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B2:O3"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="E6:K6"/>
+    <mergeCell ref="L6:O6"/>
+    <mergeCell ref="C11:C12"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3640,7 +3677,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="79" t="s">
+      <c r="A3" s="81" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -3650,7 +3687,7 @@
       <c r="D3" s="59"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="79"/>
+      <c r="A4" s="81"/>
       <c r="B4" s="1" t="s">
         <v>143</v>
       </c>
@@ -3665,7 +3702,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="79"/>
+      <c r="A5" s="81"/>
       <c r="B5" s="1" t="s">
         <v>144</v>
       </c>
@@ -3860,10 +3897,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H29"/>
+  <dimension ref="B2:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3901,7 +3938,7 @@
       </c>
     </row>
     <row r="3" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="80" t="s">
+      <c r="B3" s="92" t="s">
         <v>42</v>
       </c>
       <c r="C3" s="44" t="s">
@@ -3920,11 +3957,11 @@
       </c>
     </row>
     <row r="4" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="81"/>
-      <c r="C4" s="84" t="s">
+      <c r="B4" s="93"/>
+      <c r="C4" s="96" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="84" t="s">
+      <c r="D4" s="96" t="s">
         <v>40</v>
       </c>
       <c r="E4" s="45" t="s">
@@ -3937,9 +3974,9 @@
       </c>
     </row>
     <row r="5" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="81"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
+      <c r="B5" s="93"/>
+      <c r="C5" s="93"/>
+      <c r="D5" s="93"/>
       <c r="E5" s="45" t="s">
         <v>170</v>
       </c>
@@ -3952,9 +3989,9 @@
       </c>
     </row>
     <row r="6" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="81"/>
-      <c r="C6" s="81"/>
-      <c r="D6" s="81"/>
+      <c r="B6" s="93"/>
+      <c r="C6" s="93"/>
+      <c r="D6" s="93"/>
       <c r="E6" s="45" t="s">
         <v>171</v>
       </c>
@@ -3967,9 +4004,9 @@
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="82"/>
-      <c r="C7" s="82"/>
-      <c r="D7" s="82"/>
+      <c r="B7" s="94"/>
+      <c r="C7" s="94"/>
+      <c r="D7" s="94"/>
       <c r="E7" s="45" t="s">
         <v>41</v>
       </c>
@@ -4001,14 +4038,18 @@
         <v>180</v>
       </c>
       <c r="H8" s="45" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" s="57"/>
       <c r="C9" s="58"/>
-      <c r="D9" s="58"/>
-      <c r="E9" s="45"/>
+      <c r="D9" s="58" t="s">
+        <v>189</v>
+      </c>
+      <c r="E9" s="45" t="s">
+        <v>190</v>
+      </c>
       <c r="F9" s="45"/>
       <c r="G9" s="45"/>
       <c r="H9" s="45"/>
@@ -4032,13 +4073,13 @@
       <c r="H11" s="45"/>
     </row>
     <row r="12" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="90" t="s">
+      <c r="B12" s="84" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="85" t="s">
+      <c r="C12" s="97" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="85" t="s">
+      <c r="D12" s="97" t="s">
         <v>62</v>
       </c>
       <c r="E12" s="46" t="s">
@@ -4051,9 +4092,9 @@
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B13" s="91"/>
-      <c r="C13" s="85"/>
-      <c r="D13" s="85"/>
+      <c r="B13" s="85"/>
+      <c r="C13" s="97"/>
+      <c r="D13" s="97"/>
       <c r="E13" s="46" t="s">
         <v>61</v>
       </c>
@@ -4068,320 +4109,393 @@
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B14" s="92"/>
-      <c r="C14" s="46" t="s">
+      <c r="B14" s="85"/>
+      <c r="C14" s="63"/>
+      <c r="D14" s="63"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="63"/>
+      <c r="G14" s="63"/>
+      <c r="H14" s="63"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B15" s="86"/>
+      <c r="C15" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="D14" s="46" t="s">
+      <c r="D15" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="E14" s="46" t="s">
+      <c r="E15" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="F14" s="46" t="s">
+      <c r="F15" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="G14" s="46" t="s">
+      <c r="G15" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="H14" s="46" t="s">
+      <c r="H15" s="46" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="93" t="s">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B16" s="64"/>
+      <c r="C16" s="98"/>
+      <c r="D16" s="98" t="s">
+        <v>188</v>
+      </c>
+      <c r="E16" s="63"/>
+      <c r="F16" s="63"/>
+      <c r="G16" s="63"/>
+      <c r="H16" s="63"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B17" s="64"/>
+      <c r="C17" s="98"/>
+      <c r="D17" s="98" t="s">
+        <v>184</v>
+      </c>
+      <c r="E17" s="63"/>
+      <c r="F17" s="63"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="63"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18" s="64"/>
+      <c r="C18" s="98"/>
+      <c r="D18" s="98" t="s">
+        <v>185</v>
+      </c>
+      <c r="E18" s="63"/>
+      <c r="F18" s="63"/>
+      <c r="G18" s="63"/>
+      <c r="H18" s="63"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19" s="64"/>
+      <c r="C19" s="98"/>
+      <c r="D19" s="98" t="s">
+        <v>186</v>
+      </c>
+      <c r="E19" s="63"/>
+      <c r="F19" s="63"/>
+      <c r="G19" s="63"/>
+      <c r="H19" s="63"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20" s="64"/>
+      <c r="C20" s="98"/>
+      <c r="D20" s="98" t="s">
+        <v>187</v>
+      </c>
+      <c r="E20" s="63"/>
+      <c r="F20" s="63"/>
+      <c r="G20" s="63"/>
+      <c r="H20" s="63"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B21" s="64"/>
+      <c r="C21" s="98"/>
+      <c r="D21" s="98"/>
+      <c r="E21" s="63"/>
+      <c r="F21" s="63"/>
+      <c r="G21" s="63"/>
+      <c r="H21" s="63"/>
+    </row>
+    <row r="22" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="89" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="86" t="s">
+      <c r="C22" s="87" t="s">
         <v>71</v>
       </c>
-      <c r="D15" s="86" t="s">
+      <c r="D22" s="87" t="s">
         <v>72</v>
       </c>
-      <c r="E15" s="47" t="s">
+      <c r="E22" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="F15" s="47"/>
-      <c r="G15" s="47"/>
-      <c r="H15" s="47" t="s">
+      <c r="F22" s="47"/>
+      <c r="G22" s="47"/>
+      <c r="H22" s="47" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="94"/>
-      <c r="C16" s="87"/>
-      <c r="D16" s="87"/>
-      <c r="E16" s="47" t="s">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B23" s="90"/>
+      <c r="C23" s="88"/>
+      <c r="D23" s="88"/>
+      <c r="E23" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="F16" s="47" t="s">
-        <v>182</v>
-      </c>
-      <c r="G16" s="47" t="s">
+      <c r="F23" s="47" t="s">
+        <v>181</v>
+      </c>
+      <c r="G23" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="H16" s="48" t="s">
+      <c r="H23" s="48" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B17" s="94"/>
-      <c r="C17" s="47" t="s">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B24" s="90"/>
+      <c r="C24" s="47" t="s">
         <v>79</v>
       </c>
-      <c r="D17" s="47" t="s">
+      <c r="D24" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="E17" s="47" t="s">
+      <c r="E24" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47" t="s">
+      <c r="F24" s="47"/>
+      <c r="G24" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="H17" s="48" t="s">
+      <c r="H24" s="48" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="94"/>
-      <c r="C18" s="86" t="s">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B25" s="90"/>
+      <c r="C25" s="87" t="s">
         <v>83</v>
       </c>
-      <c r="D18" s="86" t="s">
+      <c r="D25" s="87" t="s">
         <v>84</v>
       </c>
-      <c r="E18" s="47" t="s">
+      <c r="E25" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="F18" s="47"/>
-      <c r="G18" s="47"/>
-      <c r="H18" s="47" t="s">
+      <c r="F25" s="47"/>
+      <c r="G25" s="47"/>
+      <c r="H25" s="47" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="94"/>
-      <c r="C19" s="87"/>
-      <c r="D19" s="87"/>
-      <c r="E19" s="47" t="s">
+    <row r="26" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="90"/>
+      <c r="C26" s="88"/>
+      <c r="D26" s="88"/>
+      <c r="E26" s="47" t="s">
         <v>86</v>
       </c>
-      <c r="F19" s="48" t="s">
+      <c r="F26" s="48" t="s">
         <v>106</v>
       </c>
-      <c r="G19" s="47" t="s">
+      <c r="G26" s="47" t="s">
         <v>89</v>
       </c>
-      <c r="H19" s="47" t="s">
+      <c r="H26" s="47" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="94"/>
-      <c r="C20" s="48" t="s">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B27" s="90"/>
+      <c r="C27" s="48" t="s">
         <v>94</v>
       </c>
-      <c r="D20" s="48" t="s">
+      <c r="D27" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="E20" s="48" t="s">
+      <c r="E27" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="F20" s="48"/>
-      <c r="G20" s="48" t="s">
+      <c r="F27" s="48"/>
+      <c r="G27" s="48" t="s">
         <v>95</v>
       </c>
-      <c r="H20" s="48" t="s">
+      <c r="H27" s="48" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="94"/>
-      <c r="C21" s="83" t="s">
+    <row r="28" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="90"/>
+      <c r="C28" s="95" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="83" t="s">
+      <c r="D28" s="95" t="s">
         <v>48</v>
       </c>
-      <c r="E21" s="49" t="s">
+      <c r="E28" s="49" t="s">
         <v>97</v>
       </c>
-      <c r="F21" s="49"/>
-      <c r="G21" s="50"/>
-      <c r="H21" s="49" t="s">
+      <c r="F28" s="49"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="49" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="94"/>
-      <c r="C22" s="83"/>
-      <c r="D22" s="83"/>
-      <c r="E22" s="49" t="s">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B29" s="90"/>
+      <c r="C29" s="95"/>
+      <c r="D29" s="95"/>
+      <c r="E29" s="49" t="s">
         <v>98</v>
-      </c>
-      <c r="F22" s="49" t="s">
-        <v>114</v>
-      </c>
-      <c r="G22" s="49" t="s">
-        <v>107</v>
-      </c>
-      <c r="H22" s="49"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="94"/>
-      <c r="C23" s="49" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" s="49" t="s">
-        <v>49</v>
-      </c>
-      <c r="E23" s="49" t="s">
-        <v>99</v>
-      </c>
-      <c r="F23" s="49"/>
-      <c r="G23" s="49" t="s">
-        <v>108</v>
-      </c>
-      <c r="H23" s="49" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="94"/>
-      <c r="C24" s="49" t="s">
-        <v>46</v>
-      </c>
-      <c r="D24" s="49" t="s">
-        <v>50</v>
-      </c>
-      <c r="E24" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="F24" s="49" t="s">
-        <v>183</v>
-      </c>
-      <c r="G24" s="49" t="s">
-        <v>109</v>
-      </c>
-      <c r="H24" s="49" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="94"/>
-      <c r="C25" s="88" t="s">
-        <v>47</v>
-      </c>
-      <c r="D25" s="88" t="s">
-        <v>55</v>
-      </c>
-      <c r="E25" s="49" t="s">
-        <v>101</v>
-      </c>
-      <c r="F25" s="49"/>
-      <c r="G25" s="49" t="s">
-        <v>117</v>
-      </c>
-      <c r="H25" s="49" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="94"/>
-      <c r="C26" s="89"/>
-      <c r="D26" s="89"/>
-      <c r="E26" s="49" t="s">
-        <v>102</v>
-      </c>
-      <c r="F26" s="49" t="s">
-        <v>115</v>
-      </c>
-      <c r="G26" s="49" t="s">
-        <v>110</v>
-      </c>
-      <c r="H26" s="49" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="94"/>
-      <c r="C27" s="49" t="s">
-        <v>51</v>
-      </c>
-      <c r="D27" s="49" t="s">
-        <v>54</v>
-      </c>
-      <c r="E27" s="49" t="s">
-        <v>103</v>
-      </c>
-      <c r="F27" s="49" t="s">
-        <v>184</v>
-      </c>
-      <c r="G27" s="49" t="s">
-        <v>111</v>
-      </c>
-      <c r="H27" s="51" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="94"/>
-      <c r="C28" s="88" t="s">
-        <v>52</v>
-      </c>
-      <c r="D28" s="88" t="s">
-        <v>53</v>
-      </c>
-      <c r="E28" s="49" t="s">
-        <v>104</v>
-      </c>
-      <c r="F28" s="49" t="s">
-        <v>116</v>
-      </c>
-      <c r="G28" s="49" t="s">
-        <v>112</v>
-      </c>
-      <c r="H28" s="49" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B29" s="95"/>
-      <c r="C29" s="89"/>
-      <c r="D29" s="89"/>
-      <c r="E29" s="49" t="s">
-        <v>105</v>
       </c>
       <c r="F29" s="49" t="s">
         <v>114</v>
       </c>
       <c r="G29" s="49" t="s">
+        <v>107</v>
+      </c>
+      <c r="H29" s="49"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B30" s="90"/>
+      <c r="C30" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="D30" s="49" t="s">
+        <v>49</v>
+      </c>
+      <c r="E30" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="F30" s="49"/>
+      <c r="G30" s="49" t="s">
+        <v>108</v>
+      </c>
+      <c r="H30" s="49" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B31" s="90"/>
+      <c r="C31" s="49" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" s="49" t="s">
+        <v>50</v>
+      </c>
+      <c r="E31" s="49" t="s">
+        <v>100</v>
+      </c>
+      <c r="F31" s="49" t="s">
+        <v>182</v>
+      </c>
+      <c r="G31" s="49" t="s">
+        <v>109</v>
+      </c>
+      <c r="H31" s="49" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B32" s="90"/>
+      <c r="C32" s="82" t="s">
+        <v>47</v>
+      </c>
+      <c r="D32" s="82" t="s">
+        <v>55</v>
+      </c>
+      <c r="E32" s="49" t="s">
+        <v>101</v>
+      </c>
+      <c r="F32" s="49"/>
+      <c r="G32" s="49" t="s">
+        <v>117</v>
+      </c>
+      <c r="H32" s="49" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B33" s="90"/>
+      <c r="C33" s="83"/>
+      <c r="D33" s="83"/>
+      <c r="E33" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="F33" s="49" t="s">
+        <v>115</v>
+      </c>
+      <c r="G33" s="49" t="s">
+        <v>110</v>
+      </c>
+      <c r="H33" s="49" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B34" s="90"/>
+      <c r="C34" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="D34" s="49" t="s">
+        <v>54</v>
+      </c>
+      <c r="E34" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="F34" s="49" t="s">
+        <v>183</v>
+      </c>
+      <c r="G34" s="49" t="s">
+        <v>111</v>
+      </c>
+      <c r="H34" s="51" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="90"/>
+      <c r="C35" s="82" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" s="82" t="s">
+        <v>53</v>
+      </c>
+      <c r="E35" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="F35" s="49" t="s">
+        <v>116</v>
+      </c>
+      <c r="G35" s="49" t="s">
+        <v>112</v>
+      </c>
+      <c r="H35" s="49" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B36" s="91"/>
+      <c r="C36" s="83"/>
+      <c r="D36" s="83"/>
+      <c r="E36" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="F36" s="49" t="s">
+        <v>114</v>
+      </c>
+      <c r="G36" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="H29" s="51" t="s">
+      <c r="H36" s="51" t="s">
         <v>119</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="B3:B7"/>
     <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="B15:B29"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="C21:C22"/>
     <mergeCell ref="C4:C7"/>
     <mergeCell ref="D4:D7"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="B22:B36"/>
+    <mergeCell ref="C32:C33"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Auto push 2023-03-21 18:01:47.16
</commit_message>
<xml_diff>
--- a/project/shin_movie.xlsx
+++ b/project/shin_movie.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="195">
   <si>
     <t>이용자 권한과 기능</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -170,10 +170,6 @@
   </si>
   <si>
     <t>웹페이지를 이용한 회원가입</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>join.do</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -307,18 +303,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>loginView.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>loginView.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">member/login.jsp </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>login.do</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -362,10 +346,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>member/modify.jsp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>main/main.jsp</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -505,10 +485,6 @@
   </si>
   <si>
     <t>Controller 요청 경로</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>joinView.do</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -677,18 +653,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">user/join.jsp </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>UserDto속성들</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>JoinService.java</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">adminId, adminPw </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -705,79 +673,123 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>UserEmailConfirmService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>검색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영화 검색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>searchMovie.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>movieName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SearchMovie.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userId, userPw</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boardId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boardId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영화 등록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영화 수정(개봉예정,상영작,종료)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>인물 등록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>인물 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원 제재</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>검색 결과페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>searchResult.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>searchResult.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>loginView.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>registerView.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">user/register.jsp </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>register.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">user/login.jsp </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>main/main.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user/modify.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RegisterService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>loginView.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UserIdConfirmService.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userEmail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>user/userEmailConfirm.jsp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UserIdConfirmService.java</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UserEmailConfirmService.java</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>검색</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>영화 검색</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>searchMovie.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>movieName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SearchMovie.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userId, userPw</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>boardId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>boardId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>영화 등록</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>영화 수정(개봉예정,상영작,종료)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>인물 등록</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>인물 수정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>회원 제재</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>검색 결과페이지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>searchResult.do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>searchResult.do</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1273,7 +1285,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1469,6 +1481,48 @@
     <xf numFmtId="0" fontId="11" fillId="23" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1493,33 +1547,33 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1536,12 +1590,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="21" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1550,25 +1598,7 @@
     <xf numFmtId="0" fontId="11" fillId="21" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1937,41 +1967,41 @@
     <row r="1" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
-      <c r="B2" s="66" t="s">
-        <v>134</v>
-      </c>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
-      <c r="L2" s="67"/>
-      <c r="M2" s="67"/>
-      <c r="N2" s="67"/>
-      <c r="O2" s="67"/>
+      <c r="B2" s="80" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="81"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="81"/>
+      <c r="L2" s="81"/>
+      <c r="M2" s="81"/>
+      <c r="N2" s="81"/>
+      <c r="O2" s="81"/>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="67"/>
-      <c r="L3" s="67"/>
-      <c r="M3" s="67"/>
-      <c r="N3" s="67"/>
-      <c r="O3" s="67"/>
+      <c r="B3" s="81"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="81"/>
+      <c r="M3" s="81"/>
+      <c r="N3" s="81"/>
+      <c r="O3" s="81"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
     </row>
@@ -2016,32 +2046,32 @@
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="20"/>
-      <c r="C6" s="68" t="s">
+      <c r="C6" s="82" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="39"/>
-      <c r="E6" s="70" t="s">
+      <c r="E6" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="70"/>
-      <c r="G6" s="70"/>
-      <c r="H6" s="70"/>
-      <c r="I6" s="70"/>
-      <c r="J6" s="70"/>
-      <c r="K6" s="71"/>
-      <c r="L6" s="72" t="s">
+      <c r="F6" s="84"/>
+      <c r="G6" s="84"/>
+      <c r="H6" s="84"/>
+      <c r="I6" s="84"/>
+      <c r="J6" s="84"/>
+      <c r="K6" s="85"/>
+      <c r="L6" s="86" t="s">
         <v>35</v>
       </c>
-      <c r="M6" s="70"/>
-      <c r="N6" s="70"/>
-      <c r="O6" s="70"/>
+      <c r="M6" s="84"/>
+      <c r="N6" s="84"/>
+      <c r="O6" s="84"/>
       <c r="P6" s="21"/>
       <c r="Q6" s="5"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
       <c r="B7" s="13"/>
-      <c r="C7" s="69"/>
+      <c r="C7" s="83"/>
       <c r="D7" s="22"/>
       <c r="E7" s="13">
         <v>20</v>
@@ -2141,7 +2171,7 @@
     <row r="11" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="6"/>
-      <c r="C11" s="73" t="s">
+      <c r="C11" s="76" t="s">
         <v>33</v>
       </c>
       <c r="D11" s="10"/>
@@ -2162,7 +2192,7 @@
     <row r="12" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="73"/>
+      <c r="C12" s="76"/>
       <c r="D12" s="10"/>
       <c r="E12" s="8"/>
       <c r="F12" s="6"/>
@@ -2200,7 +2230,7 @@
     <row r="14" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="6"/>
-      <c r="C14" s="65" t="s">
+      <c r="C14" s="79" t="s">
         <v>34</v>
       </c>
       <c r="D14" s="10"/>
@@ -2221,7 +2251,7 @@
     <row r="15" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="65"/>
+      <c r="C15" s="79"/>
       <c r="D15" s="10"/>
       <c r="E15" s="8"/>
       <c r="F15" s="6"/>
@@ -2259,7 +2289,7 @@
     <row r="17" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16"/>
       <c r="B17" s="6"/>
-      <c r="C17" s="73" t="s">
+      <c r="C17" s="76" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="10"/>
@@ -2280,7 +2310,7 @@
     <row r="18" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="16"/>
       <c r="B18" s="6"/>
-      <c r="C18" s="73"/>
+      <c r="C18" s="76"/>
       <c r="D18" s="10"/>
       <c r="E18" s="6"/>
       <c r="F18" s="8"/>
@@ -2339,7 +2369,7 @@
     <row r="21" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="16"/>
       <c r="B21" s="6"/>
-      <c r="C21" s="75" t="s">
+      <c r="C21" s="77" t="s">
         <v>12</v>
       </c>
       <c r="D21" s="10"/>
@@ -2360,7 +2390,7 @@
     <row r="22" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="16"/>
       <c r="B22" s="6"/>
-      <c r="C22" s="75"/>
+      <c r="C22" s="77"/>
       <c r="D22" s="10"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
@@ -2398,7 +2428,7 @@
     <row r="24" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="16"/>
       <c r="B24" s="6"/>
-      <c r="C24" s="75" t="s">
+      <c r="C24" s="77" t="s">
         <v>16</v>
       </c>
       <c r="D24" s="10"/>
@@ -2419,7 +2449,7 @@
     <row r="25" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="16"/>
       <c r="B25" s="6"/>
-      <c r="C25" s="75"/>
+      <c r="C25" s="77"/>
       <c r="D25" s="10"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
@@ -2457,8 +2487,8 @@
     <row r="27" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="16"/>
       <c r="B27" s="6"/>
-      <c r="C27" s="75" t="s">
-        <v>135</v>
+      <c r="C27" s="77" t="s">
+        <v>129</v>
       </c>
       <c r="D27" s="10"/>
       <c r="E27" s="6"/>
@@ -2478,7 +2508,7 @@
     <row r="28" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="16"/>
       <c r="B28" s="6"/>
-      <c r="C28" s="75"/>
+      <c r="C28" s="77"/>
       <c r="D28" s="10"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
@@ -2516,8 +2546,8 @@
     <row r="30" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="16"/>
       <c r="B30" s="6"/>
-      <c r="C30" s="75" t="s">
-        <v>136</v>
+      <c r="C30" s="77" t="s">
+        <v>130</v>
       </c>
       <c r="D30" s="10"/>
       <c r="E30" s="6"/>
@@ -2537,7 +2567,7 @@
     <row r="31" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="16"/>
       <c r="B31" s="6"/>
-      <c r="C31" s="75"/>
+      <c r="C31" s="77"/>
       <c r="D31" s="10"/>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
@@ -2575,8 +2605,8 @@
     <row r="33" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="16"/>
       <c r="B33" s="6"/>
-      <c r="C33" s="75" t="s">
-        <v>137</v>
+      <c r="C33" s="77" t="s">
+        <v>131</v>
       </c>
       <c r="D33" s="10"/>
       <c r="E33" s="6"/>
@@ -2596,7 +2626,7 @@
     <row r="34" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="16"/>
       <c r="B34" s="6"/>
-      <c r="C34" s="75"/>
+      <c r="C34" s="77"/>
       <c r="D34" s="10"/>
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
@@ -2674,7 +2704,7 @@
     <row r="38" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="16"/>
       <c r="B38" s="6"/>
-      <c r="C38" s="76" t="s">
+      <c r="C38" s="78" t="s">
         <v>15</v>
       </c>
       <c r="D38" s="10"/>
@@ -2695,7 +2725,7 @@
     <row r="39" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="16"/>
       <c r="B39" s="6"/>
-      <c r="C39" s="76"/>
+      <c r="C39" s="78"/>
       <c r="D39" s="10"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
@@ -2733,7 +2763,7 @@
     <row r="41" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="16"/>
       <c r="B41" s="6"/>
-      <c r="C41" s="76" t="s">
+      <c r="C41" s="78" t="s">
         <v>14</v>
       </c>
       <c r="D41" s="10"/>
@@ -2754,7 +2784,7 @@
     <row r="42" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="16"/>
       <c r="B42" s="6"/>
-      <c r="C42" s="76"/>
+      <c r="C42" s="78"/>
       <c r="D42" s="10"/>
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
@@ -2792,8 +2822,8 @@
     <row r="44" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="16"/>
       <c r="B44" s="6"/>
-      <c r="C44" s="76" t="s">
-        <v>161</v>
+      <c r="C44" s="78" t="s">
+        <v>155</v>
       </c>
       <c r="D44" s="10"/>
       <c r="E44" s="6"/>
@@ -2813,7 +2843,7 @@
     <row r="45" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="16"/>
       <c r="B45" s="6"/>
-      <c r="C45" s="76"/>
+      <c r="C45" s="78"/>
       <c r="D45" s="10"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
@@ -2851,8 +2881,8 @@
     <row r="47" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="16"/>
       <c r="B47" s="6"/>
-      <c r="C47" s="76" t="s">
-        <v>138</v>
+      <c r="C47" s="78" t="s">
+        <v>132</v>
       </c>
       <c r="D47" s="10"/>
       <c r="E47" s="6"/>
@@ -2872,7 +2902,7 @@
     <row r="48" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="16"/>
       <c r="B48" s="6"/>
-      <c r="C48" s="76"/>
+      <c r="C48" s="78"/>
       <c r="D48" s="10"/>
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
@@ -2910,8 +2940,8 @@
     <row r="50" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="16"/>
       <c r="B50" s="6"/>
-      <c r="C50" s="76" t="s">
-        <v>162</v>
+      <c r="C50" s="78" t="s">
+        <v>156</v>
       </c>
       <c r="D50" s="10"/>
       <c r="E50" s="6"/>
@@ -2931,7 +2961,7 @@
     <row r="51" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="16"/>
       <c r="B51" s="6"/>
-      <c r="C51" s="76"/>
+      <c r="C51" s="78"/>
       <c r="D51" s="10"/>
       <c r="E51" s="6"/>
       <c r="F51" s="6"/>
@@ -2990,8 +3020,8 @@
     <row r="54" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="16"/>
       <c r="B54" s="6"/>
-      <c r="C54" s="74" t="s">
-        <v>139</v>
+      <c r="C54" s="72" t="s">
+        <v>133</v>
       </c>
       <c r="D54" s="10"/>
       <c r="E54" s="6"/>
@@ -3011,7 +3041,7 @@
     <row r="55" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="16"/>
       <c r="B55" s="6"/>
-      <c r="C55" s="74"/>
+      <c r="C55" s="72"/>
       <c r="D55" s="10"/>
       <c r="E55" s="6"/>
       <c r="F55" s="6"/>
@@ -3049,8 +3079,8 @@
     <row r="57" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="16"/>
       <c r="B57" s="6"/>
-      <c r="C57" s="74" t="s">
-        <v>140</v>
+      <c r="C57" s="72" t="s">
+        <v>134</v>
       </c>
       <c r="D57" s="10"/>
       <c r="E57" s="6"/>
@@ -3070,7 +3100,7 @@
     <row r="58" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="16"/>
       <c r="B58" s="6"/>
-      <c r="C58" s="74"/>
+      <c r="C58" s="72"/>
       <c r="D58" s="10"/>
       <c r="E58" s="6"/>
       <c r="F58" s="6"/>
@@ -3108,8 +3138,8 @@
     <row r="60" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="16"/>
       <c r="B60" s="6"/>
-      <c r="C60" s="74" t="s">
-        <v>160</v>
+      <c r="C60" s="72" t="s">
+        <v>154</v>
       </c>
       <c r="D60" s="10"/>
       <c r="E60" s="6"/>
@@ -3129,7 +3159,7 @@
     <row r="61" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="16"/>
       <c r="B61" s="6"/>
-      <c r="C61" s="74"/>
+      <c r="C61" s="72"/>
       <c r="D61" s="10"/>
       <c r="E61" s="6"/>
       <c r="F61" s="6"/>
@@ -3167,8 +3197,8 @@
     <row r="63" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="16"/>
       <c r="B63" s="6"/>
-      <c r="C63" s="74" t="s">
-        <v>159</v>
+      <c r="C63" s="72" t="s">
+        <v>153</v>
       </c>
       <c r="D63" s="10"/>
       <c r="E63" s="6"/>
@@ -3188,7 +3218,7 @@
     <row r="64" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="16"/>
       <c r="B64" s="6"/>
-      <c r="C64" s="74"/>
+      <c r="C64" s="72"/>
       <c r="D64" s="10"/>
       <c r="E64" s="6"/>
       <c r="F64" s="6"/>
@@ -3226,8 +3256,8 @@
     <row r="66" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="16"/>
       <c r="B66" s="6"/>
-      <c r="C66" s="74" t="s">
-        <v>158</v>
+      <c r="C66" s="72" t="s">
+        <v>152</v>
       </c>
       <c r="D66" s="10"/>
       <c r="E66" s="6"/>
@@ -3247,7 +3277,7 @@
     <row r="67" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="16"/>
       <c r="B67" s="6"/>
-      <c r="C67" s="74"/>
+      <c r="C67" s="72"/>
       <c r="D67" s="10"/>
       <c r="E67" s="6"/>
       <c r="F67" s="6"/>
@@ -3285,8 +3315,8 @@
     <row r="69" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="16"/>
       <c r="B69" s="6"/>
-      <c r="C69" s="74" t="s">
-        <v>157</v>
+      <c r="C69" s="72" t="s">
+        <v>151</v>
       </c>
       <c r="D69" s="10"/>
       <c r="E69" s="6"/>
@@ -3306,7 +3336,7 @@
     <row r="70" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="16"/>
       <c r="B70" s="6"/>
-      <c r="C70" s="74"/>
+      <c r="C70" s="72"/>
       <c r="D70" s="10"/>
       <c r="E70" s="6"/>
       <c r="F70" s="6"/>
@@ -3344,8 +3374,8 @@
     <row r="72" spans="1:68" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="16"/>
       <c r="B72" s="6"/>
-      <c r="C72" s="78" t="s">
-        <v>57</v>
+      <c r="C72" s="73" t="s">
+        <v>56</v>
       </c>
       <c r="D72" s="7"/>
       <c r="E72" s="6"/>
@@ -3365,7 +3395,7 @@
     <row r="73" spans="1:68" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="16"/>
       <c r="B73" s="6"/>
-      <c r="C73" s="78"/>
+      <c r="C73" s="73"/>
       <c r="D73" s="7"/>
       <c r="E73" s="6"/>
       <c r="F73" s="6"/>
@@ -3384,8 +3414,8 @@
     <row r="74" spans="1:68" s="5" customFormat="1" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="16"/>
       <c r="B74" s="6"/>
-      <c r="C74" s="80" t="s">
-        <v>133</v>
+      <c r="C74" s="75" t="s">
+        <v>127</v>
       </c>
       <c r="D74" s="7"/>
       <c r="E74" s="6"/>
@@ -3455,7 +3485,7 @@
     <row r="75" spans="1:68" s="5" customFormat="1" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="16"/>
       <c r="B75" s="6"/>
-      <c r="C75" s="80"/>
+      <c r="C75" s="75"/>
       <c r="D75" s="7"/>
       <c r="E75" s="6"/>
       <c r="F75" s="6"/>
@@ -3583,18 +3613,18 @@
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
       <c r="E79" s="5"/>
-      <c r="F79" s="79"/>
-      <c r="G79" s="79"/>
+      <c r="F79" s="74"/>
+      <c r="G79" s="74"/>
       <c r="H79" s="6"/>
       <c r="I79" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J79" s="38"/>
       <c r="K79" s="6"/>
-      <c r="L79" s="77" t="s">
-        <v>58</v>
-      </c>
-      <c r="M79" s="77"/>
+      <c r="L79" s="71" t="s">
+        <v>57</v>
+      </c>
+      <c r="M79" s="71"/>
       <c r="N79" s="40"/>
       <c r="O79" s="5"/>
       <c r="P79" s="5"/>
@@ -3620,15 +3650,12 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="L79:M79"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="F79:G79"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="C69:C70"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B2:O3"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="E6:K6"/>
+    <mergeCell ref="L6:O6"/>
+    <mergeCell ref="C11:C12"/>
     <mergeCell ref="C54:C55"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="C21:C22"/>
@@ -3641,12 +3668,15 @@
     <mergeCell ref="C44:C45"/>
     <mergeCell ref="C50:C51"/>
     <mergeCell ref="C47:C48"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="B2:O3"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="E6:K6"/>
-    <mergeCell ref="L6:O6"/>
-    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="L79:M79"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="F79:G79"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="C69:C70"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3677,46 +3707,46 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="81" t="s">
+      <c r="A3" s="87" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C3" s="59"/>
       <c r="D3" s="59"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="81"/>
+      <c r="A4" s="87"/>
       <c r="B4" s="1" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="81"/>
+      <c r="A5" s="87"/>
       <c r="B5" s="1" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -3730,19 +3760,19 @@
         <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="F6" s="62" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -3775,24 +3805,24 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C2" s="61"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C3" s="60"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C19" s="56"/>
     </row>
@@ -3897,10 +3927,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H36"/>
+  <dimension ref="B2:H48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3919,151 +3949,155 @@
     <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B2" s="41"/>
       <c r="C2" s="42" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D2" s="42" t="s">
         <v>36</v>
       </c>
       <c r="E2" s="42" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="F2" s="42" t="s">
         <v>37</v>
       </c>
       <c r="G2" s="42" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="H2" s="42" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="3" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="92" t="s">
-        <v>42</v>
+      <c r="B3" s="88" t="s">
+        <v>41</v>
       </c>
       <c r="C3" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="44" t="s">
+      <c r="E3" s="45" t="s">
         <v>68</v>
-      </c>
-      <c r="E3" s="45" t="s">
-        <v>69</v>
       </c>
       <c r="F3" s="45"/>
       <c r="G3" s="45"/>
       <c r="H3" s="45" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="93"/>
-      <c r="C4" s="96" t="s">
+      <c r="B4" s="89"/>
+      <c r="C4" s="92" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="96" t="s">
+      <c r="D4" s="92" t="s">
         <v>40</v>
       </c>
       <c r="E4" s="45" t="s">
-        <v>124</v>
+        <v>183</v>
       </c>
       <c r="F4" s="45"/>
       <c r="G4" s="45"/>
       <c r="H4" s="45" t="s">
-        <v>166</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="93"/>
-      <c r="C5" s="93"/>
-      <c r="D5" s="93"/>
+      <c r="B5" s="89"/>
+      <c r="C5" s="89"/>
+      <c r="D5" s="89"/>
       <c r="E5" s="45" t="s">
-        <v>170</v>
-      </c>
-      <c r="F5" s="45"/>
+        <v>162</v>
+      </c>
+      <c r="F5" s="45" t="s">
+        <v>191</v>
+      </c>
       <c r="G5" s="45" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="H5" s="45" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="93"/>
-      <c r="C6" s="93"/>
-      <c r="D6" s="93"/>
+      <c r="B6" s="89"/>
+      <c r="C6" s="89"/>
+      <c r="D6" s="89"/>
       <c r="E6" s="45" t="s">
-        <v>171</v>
-      </c>
-      <c r="F6" s="45"/>
+        <v>163</v>
+      </c>
+      <c r="F6" s="45" t="s">
+        <v>193</v>
+      </c>
       <c r="G6" s="45" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="H6" s="45" t="s">
-        <v>173</v>
+        <v>194</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="94"/>
-      <c r="C7" s="94"/>
-      <c r="D7" s="94"/>
+      <c r="B7" s="90"/>
+      <c r="C7" s="90"/>
+      <c r="D7" s="90"/>
       <c r="E7" s="45" t="s">
-        <v>41</v>
+        <v>185</v>
       </c>
       <c r="F7" s="45" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="G7" s="45" t="s">
-        <v>168</v>
+        <v>189</v>
       </c>
       <c r="H7" s="45" t="s">
-        <v>73</v>
+        <v>190</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="57"/>
       <c r="C8" s="58" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="D8" s="58" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="E8" s="45" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="F8" s="45" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="G8" s="45" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="H8" s="45" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" s="57"/>
       <c r="C9" s="58"/>
       <c r="D9" s="58" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="E9" s="45" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="F9" s="45"/>
       <c r="G9" s="45"/>
       <c r="H9" s="45"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="57"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58"/>
+      <c r="B10" s="67"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="68"/>
       <c r="E10" s="45"/>
       <c r="F10" s="45"/>
       <c r="G10" s="45"/>
       <c r="H10" s="45"/>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="57"/>
       <c r="C11" s="58"/>
       <c r="D11" s="58"/>
@@ -4072,430 +4106,538 @@
       <c r="G11" s="45"/>
       <c r="H11" s="45"/>
     </row>
-    <row r="12" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="84" t="s">
-        <v>56</v>
-      </c>
-      <c r="C12" s="97" t="s">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B12" s="57"/>
+      <c r="C12" s="58"/>
+      <c r="D12" s="58"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="45"/>
+    </row>
+    <row r="13" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="101" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="94" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="94" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13" s="47" t="s">
+        <v>182</v>
+      </c>
+      <c r="F13" s="47"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="47" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B14" s="102"/>
+      <c r="C14" s="95"/>
+      <c r="D14" s="95"/>
+      <c r="E14" s="47" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" s="47" t="s">
+        <v>171</v>
+      </c>
+      <c r="G14" s="47" t="s">
+        <v>73</v>
+      </c>
+      <c r="H14" s="48" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B15" s="102"/>
+      <c r="C15" s="47" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" s="47"/>
+      <c r="G15" s="47" t="s">
+        <v>78</v>
+      </c>
+      <c r="H15" s="48" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B16" s="102"/>
+      <c r="C16" s="94" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" s="94" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" s="47" t="s">
+        <v>81</v>
+      </c>
+      <c r="F16" s="47"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="47" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="102"/>
+      <c r="C17" s="95"/>
+      <c r="D17" s="95"/>
+      <c r="E17" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="F17" s="48" t="s">
+        <v>101</v>
+      </c>
+      <c r="G17" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="H17" s="47" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="102"/>
+      <c r="C18" s="66"/>
+      <c r="D18" s="66"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="48"/>
+      <c r="H18" s="48"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19" s="102"/>
+      <c r="C19" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="D19" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="E19" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="F19" s="48"/>
+      <c r="G19" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="H19" s="48" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20" s="102"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="48"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="104"/>
+      <c r="H20" s="48"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B21" s="102"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="48"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="104"/>
+      <c r="H21" s="48"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B22" s="102"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="48"/>
+      <c r="E22" s="48"/>
+      <c r="F22" s="48"/>
+      <c r="G22" s="104"/>
+      <c r="H22" s="48"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B23" s="102"/>
+      <c r="C23" s="48"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="48"/>
+      <c r="F23" s="48"/>
+      <c r="G23" s="104"/>
+      <c r="H23" s="48"/>
+    </row>
+    <row r="24" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="102"/>
+      <c r="C24" s="91" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="91" t="s">
+        <v>47</v>
+      </c>
+      <c r="E24" s="49" t="s">
+        <v>92</v>
+      </c>
+      <c r="F24" s="49"/>
+      <c r="G24" s="50"/>
+      <c r="H24" s="49" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B25" s="102"/>
+      <c r="C25" s="91"/>
+      <c r="D25" s="91"/>
+      <c r="E25" s="49" t="s">
+        <v>93</v>
+      </c>
+      <c r="F25" s="49" t="s">
+        <v>109</v>
+      </c>
+      <c r="G25" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="H25" s="49"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B26" s="102"/>
+      <c r="C26" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" s="49" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" s="49" t="s">
+        <v>94</v>
+      </c>
+      <c r="F26" s="49"/>
+      <c r="G26" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="H26" s="49" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B27" s="102"/>
+      <c r="C27" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" s="49" t="s">
+        <v>49</v>
+      </c>
+      <c r="E27" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="F27" s="49" t="s">
+        <v>172</v>
+      </c>
+      <c r="G27" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="H27" s="49" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B28" s="102"/>
+      <c r="C28" s="96" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="E28" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="F28" s="49"/>
+      <c r="G28" s="49" t="s">
+        <v>112</v>
+      </c>
+      <c r="H28" s="49" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B29" s="102"/>
+      <c r="C29" s="97"/>
+      <c r="D29" s="97"/>
+      <c r="E29" s="49" t="s">
+        <v>97</v>
+      </c>
+      <c r="F29" s="49" t="s">
+        <v>110</v>
+      </c>
+      <c r="G29" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="H29" s="49" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B30" s="102"/>
+      <c r="C30" s="49" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="E30" s="49" t="s">
+        <v>98</v>
+      </c>
+      <c r="F30" s="49" t="s">
+        <v>173</v>
+      </c>
+      <c r="G30" s="49" t="s">
+        <v>106</v>
+      </c>
+      <c r="H30" s="51" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B31" s="102"/>
+      <c r="C31" s="65"/>
+      <c r="D31" s="65"/>
+      <c r="E31" s="69"/>
+      <c r="F31" s="69"/>
+      <c r="G31" s="69"/>
+      <c r="H31" s="69"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B32" s="102"/>
+      <c r="C32" s="65"/>
+      <c r="D32" s="65"/>
+      <c r="E32" s="69"/>
+      <c r="F32" s="69"/>
+      <c r="G32" s="69"/>
+      <c r="H32" s="69"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B33" s="102"/>
+      <c r="C33" s="65"/>
+      <c r="D33" s="65"/>
+      <c r="E33" s="69"/>
+      <c r="F33" s="69"/>
+      <c r="G33" s="69"/>
+      <c r="H33" s="69"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B34" s="102"/>
+      <c r="C34" s="65"/>
+      <c r="D34" s="65"/>
+      <c r="E34" s="69"/>
+      <c r="F34" s="69"/>
+      <c r="G34" s="69"/>
+      <c r="H34" s="69"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B35" s="102"/>
+      <c r="C35" s="65"/>
+      <c r="D35" s="65"/>
+      <c r="E35" s="69"/>
+      <c r="F35" s="69"/>
+      <c r="G35" s="69"/>
+      <c r="H35" s="69"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B36" s="102"/>
+      <c r="C36" s="65"/>
+      <c r="D36" s="65"/>
+      <c r="E36" s="69"/>
+      <c r="F36" s="69"/>
+      <c r="G36" s="69"/>
+      <c r="H36" s="69"/>
+    </row>
+    <row r="37" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="102"/>
+      <c r="C37" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="D37" s="96" t="s">
+        <v>52</v>
+      </c>
+      <c r="E37" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="F37" s="49" t="s">
+        <v>111</v>
+      </c>
+      <c r="G37" s="49" t="s">
+        <v>107</v>
+      </c>
+      <c r="H37" s="49" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B38" s="103"/>
+      <c r="C38" s="97"/>
+      <c r="D38" s="97"/>
+      <c r="E38" s="49" t="s">
+        <v>100</v>
+      </c>
+      <c r="F38" s="49" t="s">
+        <v>109</v>
+      </c>
+      <c r="G38" s="49" t="s">
+        <v>108</v>
+      </c>
+      <c r="H38" s="51" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B39" s="98" t="s">
+        <v>55</v>
+      </c>
+      <c r="C39" s="93" t="s">
+        <v>59</v>
+      </c>
+      <c r="D39" s="93" t="s">
+        <v>61</v>
+      </c>
+      <c r="E39" s="46" t="s">
+        <v>119</v>
+      </c>
+      <c r="F39" s="46"/>
+      <c r="G39" s="46"/>
+      <c r="H39" s="46" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B40" s="99"/>
+      <c r="C40" s="93"/>
+      <c r="D40" s="93"/>
+      <c r="E40" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="97" t="s">
+      <c r="F40" s="46" t="s">
+        <v>161</v>
+      </c>
+      <c r="G40" s="46" t="s">
+        <v>121</v>
+      </c>
+      <c r="H40" s="46" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B41" s="99"/>
+      <c r="C41" s="63"/>
+      <c r="D41" s="63"/>
+      <c r="E41" s="63"/>
+      <c r="F41" s="63"/>
+      <c r="G41" s="63"/>
+      <c r="H41" s="63"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B42" s="100"/>
+      <c r="C42" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="E12" s="46" t="s">
-        <v>125</v>
-      </c>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="46" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B13" s="85"/>
-      <c r="C13" s="97"/>
-      <c r="D13" s="97"/>
-      <c r="E13" s="46" t="s">
-        <v>61</v>
-      </c>
-      <c r="F13" s="46" t="s">
-        <v>169</v>
-      </c>
-      <c r="G13" s="46" t="s">
-        <v>127</v>
-      </c>
-      <c r="H13" s="46" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B14" s="85"/>
-      <c r="C14" s="63"/>
-      <c r="D14" s="63"/>
-      <c r="E14" s="63"/>
-      <c r="F14" s="63"/>
-      <c r="G14" s="63"/>
-      <c r="H14" s="63"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B15" s="86"/>
-      <c r="C15" s="46" t="s">
+      <c r="D42" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="46" t="s">
+      <c r="E42" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="E15" s="46" t="s">
+      <c r="F42" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="F15" s="46" t="s">
-        <v>66</v>
-      </c>
-      <c r="G15" s="46" t="s">
-        <v>90</v>
-      </c>
-      <c r="H15" s="46" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="64"/>
-      <c r="C16" s="98"/>
-      <c r="D16" s="98" t="s">
-        <v>188</v>
-      </c>
-      <c r="E16" s="63"/>
-      <c r="F16" s="63"/>
-      <c r="G16" s="63"/>
-      <c r="H16" s="63"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B17" s="64"/>
-      <c r="C17" s="98"/>
-      <c r="D17" s="98" t="s">
-        <v>184</v>
-      </c>
-      <c r="E17" s="63"/>
-      <c r="F17" s="63"/>
-      <c r="G17" s="63"/>
-      <c r="H17" s="63"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="64"/>
-      <c r="C18" s="98"/>
-      <c r="D18" s="98" t="s">
-        <v>185</v>
-      </c>
-      <c r="E18" s="63"/>
-      <c r="F18" s="63"/>
-      <c r="G18" s="63"/>
-      <c r="H18" s="63"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="64"/>
-      <c r="C19" s="98"/>
-      <c r="D19" s="98" t="s">
-        <v>186</v>
-      </c>
-      <c r="E19" s="63"/>
-      <c r="F19" s="63"/>
-      <c r="G19" s="63"/>
-      <c r="H19" s="63"/>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="64"/>
-      <c r="C20" s="98"/>
-      <c r="D20" s="98" t="s">
-        <v>187</v>
-      </c>
-      <c r="E20" s="63"/>
-      <c r="F20" s="63"/>
-      <c r="G20" s="63"/>
-      <c r="H20" s="63"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="64"/>
-      <c r="C21" s="98"/>
-      <c r="D21" s="98"/>
-      <c r="E21" s="63"/>
-      <c r="F21" s="63"/>
-      <c r="G21" s="63"/>
-      <c r="H21" s="63"/>
-    </row>
-    <row r="22" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="89" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" s="87" t="s">
-        <v>71</v>
-      </c>
-      <c r="D22" s="87" t="s">
-        <v>72</v>
-      </c>
-      <c r="E22" s="47" t="s">
-        <v>74</v>
-      </c>
-      <c r="F22" s="47"/>
-      <c r="G22" s="47"/>
-      <c r="H22" s="47" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="90"/>
-      <c r="C23" s="88"/>
-      <c r="D23" s="88"/>
-      <c r="E23" s="47" t="s">
-        <v>76</v>
-      </c>
-      <c r="F23" s="47" t="s">
-        <v>181</v>
-      </c>
-      <c r="G23" s="47" t="s">
-        <v>77</v>
-      </c>
-      <c r="H23" s="48" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="90"/>
-      <c r="C24" s="47" t="s">
-        <v>79</v>
-      </c>
-      <c r="D24" s="47" t="s">
-        <v>80</v>
-      </c>
-      <c r="E24" s="47" t="s">
-        <v>81</v>
-      </c>
-      <c r="F24" s="47"/>
-      <c r="G24" s="47" t="s">
-        <v>82</v>
-      </c>
-      <c r="H24" s="48" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="90"/>
-      <c r="C25" s="87" t="s">
-        <v>83</v>
-      </c>
-      <c r="D25" s="87" t="s">
-        <v>84</v>
-      </c>
-      <c r="E25" s="47" t="s">
+      <c r="G42" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="F25" s="47"/>
-      <c r="G25" s="47"/>
-      <c r="H25" s="47" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="90"/>
-      <c r="C26" s="88"/>
-      <c r="D26" s="88"/>
-      <c r="E26" s="47" t="s">
-        <v>86</v>
-      </c>
-      <c r="F26" s="48" t="s">
-        <v>106</v>
-      </c>
-      <c r="G26" s="47" t="s">
-        <v>89</v>
-      </c>
-      <c r="H26" s="47" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="90"/>
-      <c r="C27" s="48" t="s">
-        <v>94</v>
-      </c>
-      <c r="D27" s="48" t="s">
-        <v>93</v>
-      </c>
-      <c r="E27" s="48" t="s">
-        <v>92</v>
-      </c>
-      <c r="F27" s="48"/>
-      <c r="G27" s="48" t="s">
-        <v>95</v>
-      </c>
-      <c r="H27" s="48" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="90"/>
-      <c r="C28" s="95" t="s">
-        <v>44</v>
-      </c>
-      <c r="D28" s="95" t="s">
-        <v>48</v>
-      </c>
-      <c r="E28" s="49" t="s">
-        <v>97</v>
-      </c>
-      <c r="F28" s="49"/>
-      <c r="G28" s="50"/>
-      <c r="H28" s="49" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B29" s="90"/>
-      <c r="C29" s="95"/>
-      <c r="D29" s="95"/>
-      <c r="E29" s="49" t="s">
-        <v>98</v>
-      </c>
-      <c r="F29" s="49" t="s">
-        <v>114</v>
-      </c>
-      <c r="G29" s="49" t="s">
-        <v>107</v>
-      </c>
-      <c r="H29" s="49"/>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B30" s="90"/>
-      <c r="C30" s="49" t="s">
-        <v>45</v>
-      </c>
-      <c r="D30" s="49" t="s">
-        <v>49</v>
-      </c>
-      <c r="E30" s="49" t="s">
-        <v>99</v>
-      </c>
-      <c r="F30" s="49"/>
-      <c r="G30" s="49" t="s">
-        <v>108</v>
-      </c>
-      <c r="H30" s="49" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B31" s="90"/>
-      <c r="C31" s="49" t="s">
-        <v>46</v>
-      </c>
-      <c r="D31" s="49" t="s">
-        <v>50</v>
-      </c>
-      <c r="E31" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="F31" s="49" t="s">
-        <v>182</v>
-      </c>
-      <c r="G31" s="49" t="s">
-        <v>109</v>
-      </c>
-      <c r="H31" s="49" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B32" s="90"/>
-      <c r="C32" s="82" t="s">
-        <v>47</v>
-      </c>
-      <c r="D32" s="82" t="s">
-        <v>55</v>
-      </c>
-      <c r="E32" s="49" t="s">
-        <v>101</v>
-      </c>
-      <c r="F32" s="49"/>
-      <c r="G32" s="49" t="s">
-        <v>117</v>
-      </c>
-      <c r="H32" s="49" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B33" s="90"/>
-      <c r="C33" s="83"/>
-      <c r="D33" s="83"/>
-      <c r="E33" s="49" t="s">
-        <v>102</v>
-      </c>
-      <c r="F33" s="49" t="s">
-        <v>115</v>
-      </c>
-      <c r="G33" s="49" t="s">
-        <v>110</v>
-      </c>
-      <c r="H33" s="49" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B34" s="90"/>
-      <c r="C34" s="49" t="s">
-        <v>51</v>
-      </c>
-      <c r="D34" s="49" t="s">
-        <v>54</v>
-      </c>
-      <c r="E34" s="49" t="s">
-        <v>103</v>
-      </c>
-      <c r="F34" s="49" t="s">
-        <v>183</v>
-      </c>
-      <c r="G34" s="49" t="s">
-        <v>111</v>
-      </c>
-      <c r="H34" s="51" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="90"/>
-      <c r="C35" s="82" t="s">
-        <v>52</v>
-      </c>
-      <c r="D35" s="82" t="s">
-        <v>53</v>
-      </c>
-      <c r="E35" s="49" t="s">
-        <v>104</v>
-      </c>
-      <c r="F35" s="49" t="s">
-        <v>116</v>
-      </c>
-      <c r="G35" s="49" t="s">
-        <v>112</v>
-      </c>
-      <c r="H35" s="49" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B36" s="91"/>
-      <c r="C36" s="83"/>
-      <c r="D36" s="83"/>
-      <c r="E36" s="49" t="s">
-        <v>105</v>
-      </c>
-      <c r="F36" s="49" t="s">
-        <v>114</v>
-      </c>
-      <c r="G36" s="49" t="s">
+      <c r="H42" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="H36" s="51" t="s">
-        <v>119</v>
-      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B43" s="64"/>
+      <c r="C43" s="70"/>
+      <c r="D43" s="70" t="s">
+        <v>178</v>
+      </c>
+      <c r="E43" s="63"/>
+      <c r="F43" s="63"/>
+      <c r="G43" s="63"/>
+      <c r="H43" s="63"/>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B44" s="64"/>
+      <c r="C44" s="70"/>
+      <c r="D44" s="70" t="s">
+        <v>174</v>
+      </c>
+      <c r="E44" s="63"/>
+      <c r="F44" s="63"/>
+      <c r="G44" s="63"/>
+      <c r="H44" s="63"/>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B45" s="64"/>
+      <c r="C45" s="70"/>
+      <c r="D45" s="70" t="s">
+        <v>175</v>
+      </c>
+      <c r="E45" s="63"/>
+      <c r="F45" s="63"/>
+      <c r="G45" s="63"/>
+      <c r="H45" s="63"/>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B46" s="64"/>
+      <c r="C46" s="70"/>
+      <c r="D46" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="E46" s="63"/>
+      <c r="F46" s="63"/>
+      <c r="G46" s="63"/>
+      <c r="H46" s="63"/>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B47" s="64"/>
+      <c r="C47" s="70"/>
+      <c r="D47" s="70" t="s">
+        <v>177</v>
+      </c>
+      <c r="E47" s="63"/>
+      <c r="F47" s="63"/>
+      <c r="G47" s="63"/>
+      <c r="H47" s="63"/>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B48" s="64"/>
+      <c r="C48" s="70"/>
+      <c r="D48" s="70"/>
+      <c r="E48" s="63"/>
+      <c r="F48" s="63"/>
+      <c r="G48" s="63"/>
+      <c r="H48" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="B13:B38"/>
+    <mergeCell ref="C28:C29"/>
     <mergeCell ref="B3:B7"/>
-    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C24:C25"/>
     <mergeCell ref="C4:C7"/>
     <mergeCell ref="D4:D7"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="B22:B36"/>
-    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D24:D25"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Auto push 2023-03-22 18:01:25.72
</commit_message>
<xml_diff>
--- a/project/shin_movie.xlsx
+++ b/project/shin_movie.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="207">
   <si>
     <t>이용자 권한과 기능</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -790,6 +790,54 @@
   </si>
   <si>
     <t>user/userEmailConfirm.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ppt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IMDb 헤더색상 18 18 18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IMDb 카드리스트2  44 44 44</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IMDb 카드리스트1  26 26 26</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리얼블랙 0 0 0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100 100 100   64 64 64</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0 0 0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>75 75 75   4b 4b 4b</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>44 44 44 2c2c2c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>130 130 130   82 82 82</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>배경</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그라데이션 로그인</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -895,7 +943,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="29">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1061,6 +1109,48 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF0A0A0A"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF121212"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF1A1A1A"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2C2C2C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF828282"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF646464"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4B4B4B"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1285,7 +1375,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1499,6 +1589,12 @@
     <xf numFmtId="0" fontId="11" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1598,8 +1694,23 @@
     <xf numFmtId="0" fontId="11" fillId="21" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1637,16 +1748,16 @@
   </tableStyles>
   <colors>
     <mruColors>
+      <color rgb="FF2C2C2C"/>
+      <color rgb="FF4B4B4B"/>
+      <color rgb="FF646464"/>
+      <color rgb="FF828282"/>
+      <color rgb="FF1A1A1A"/>
+      <color rgb="FF121212"/>
       <color rgb="FF0A0A0A"/>
       <color rgb="FF373737"/>
       <color rgb="FF3FFFDA"/>
       <color rgb="FFFFFFCC"/>
-      <color rgb="FFFFFFFF"/>
-      <color rgb="FFE1FFE1"/>
-      <color rgb="FFFFFFDD"/>
-      <color rgb="FFF1F5E7"/>
-      <color rgb="FFFFDDFF"/>
-      <color rgb="FFE5F4F7"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1967,41 +2078,41 @@
     <row r="1" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="82" t="s">
         <v>128</v>
       </c>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
-      <c r="L2" s="81"/>
-      <c r="M2" s="81"/>
-      <c r="N2" s="81"/>
-      <c r="O2" s="81"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="83"/>
+      <c r="N2" s="83"/>
+      <c r="O2" s="83"/>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
-      <c r="B3" s="81"/>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="81"/>
-      <c r="O3" s="81"/>
+      <c r="B3" s="83"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="83"/>
+      <c r="F3" s="83"/>
+      <c r="G3" s="83"/>
+      <c r="H3" s="83"/>
+      <c r="I3" s="83"/>
+      <c r="J3" s="83"/>
+      <c r="K3" s="83"/>
+      <c r="L3" s="83"/>
+      <c r="M3" s="83"/>
+      <c r="N3" s="83"/>
+      <c r="O3" s="83"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
     </row>
@@ -2046,32 +2157,32 @@
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="20"/>
-      <c r="C6" s="82" t="s">
+      <c r="C6" s="84" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="39"/>
-      <c r="E6" s="84" t="s">
+      <c r="E6" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="84"/>
-      <c r="G6" s="84"/>
-      <c r="H6" s="84"/>
-      <c r="I6" s="84"/>
-      <c r="J6" s="84"/>
-      <c r="K6" s="85"/>
-      <c r="L6" s="86" t="s">
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
+      <c r="H6" s="86"/>
+      <c r="I6" s="86"/>
+      <c r="J6" s="86"/>
+      <c r="K6" s="87"/>
+      <c r="L6" s="88" t="s">
         <v>35</v>
       </c>
-      <c r="M6" s="84"/>
-      <c r="N6" s="84"/>
-      <c r="O6" s="84"/>
+      <c r="M6" s="86"/>
+      <c r="N6" s="86"/>
+      <c r="O6" s="86"/>
       <c r="P6" s="21"/>
       <c r="Q6" s="5"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
       <c r="B7" s="13"/>
-      <c r="C7" s="83"/>
+      <c r="C7" s="85"/>
       <c r="D7" s="22"/>
       <c r="E7" s="13">
         <v>20</v>
@@ -2171,7 +2282,7 @@
     <row r="11" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="6"/>
-      <c r="C11" s="76" t="s">
+      <c r="C11" s="78" t="s">
         <v>33</v>
       </c>
       <c r="D11" s="10"/>
@@ -2192,7 +2303,7 @@
     <row r="12" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="76"/>
+      <c r="C12" s="78"/>
       <c r="D12" s="10"/>
       <c r="E12" s="8"/>
       <c r="F12" s="6"/>
@@ -2230,7 +2341,7 @@
     <row r="14" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="6"/>
-      <c r="C14" s="79" t="s">
+      <c r="C14" s="81" t="s">
         <v>34</v>
       </c>
       <c r="D14" s="10"/>
@@ -2251,7 +2362,7 @@
     <row r="15" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="79"/>
+      <c r="C15" s="81"/>
       <c r="D15" s="10"/>
       <c r="E15" s="8"/>
       <c r="F15" s="6"/>
@@ -2289,7 +2400,7 @@
     <row r="17" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16"/>
       <c r="B17" s="6"/>
-      <c r="C17" s="76" t="s">
+      <c r="C17" s="78" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="10"/>
@@ -2310,7 +2421,7 @@
     <row r="18" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="16"/>
       <c r="B18" s="6"/>
-      <c r="C18" s="76"/>
+      <c r="C18" s="78"/>
       <c r="D18" s="10"/>
       <c r="E18" s="6"/>
       <c r="F18" s="8"/>
@@ -2369,7 +2480,7 @@
     <row r="21" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="16"/>
       <c r="B21" s="6"/>
-      <c r="C21" s="77" t="s">
+      <c r="C21" s="79" t="s">
         <v>12</v>
       </c>
       <c r="D21" s="10"/>
@@ -2390,7 +2501,7 @@
     <row r="22" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="16"/>
       <c r="B22" s="6"/>
-      <c r="C22" s="77"/>
+      <c r="C22" s="79"/>
       <c r="D22" s="10"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
@@ -2428,7 +2539,7 @@
     <row r="24" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="16"/>
       <c r="B24" s="6"/>
-      <c r="C24" s="77" t="s">
+      <c r="C24" s="79" t="s">
         <v>16</v>
       </c>
       <c r="D24" s="10"/>
@@ -2449,7 +2560,7 @@
     <row r="25" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="16"/>
       <c r="B25" s="6"/>
-      <c r="C25" s="77"/>
+      <c r="C25" s="79"/>
       <c r="D25" s="10"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
@@ -2487,7 +2598,7 @@
     <row r="27" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="16"/>
       <c r="B27" s="6"/>
-      <c r="C27" s="77" t="s">
+      <c r="C27" s="79" t="s">
         <v>129</v>
       </c>
       <c r="D27" s="10"/>
@@ -2508,7 +2619,7 @@
     <row r="28" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="16"/>
       <c r="B28" s="6"/>
-      <c r="C28" s="77"/>
+      <c r="C28" s="79"/>
       <c r="D28" s="10"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
@@ -2546,7 +2657,7 @@
     <row r="30" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="16"/>
       <c r="B30" s="6"/>
-      <c r="C30" s="77" t="s">
+      <c r="C30" s="79" t="s">
         <v>130</v>
       </c>
       <c r="D30" s="10"/>
@@ -2567,7 +2678,7 @@
     <row r="31" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="16"/>
       <c r="B31" s="6"/>
-      <c r="C31" s="77"/>
+      <c r="C31" s="79"/>
       <c r="D31" s="10"/>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
@@ -2605,7 +2716,7 @@
     <row r="33" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="16"/>
       <c r="B33" s="6"/>
-      <c r="C33" s="77" t="s">
+      <c r="C33" s="79" t="s">
         <v>131</v>
       </c>
       <c r="D33" s="10"/>
@@ -2626,7 +2737,7 @@
     <row r="34" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="16"/>
       <c r="B34" s="6"/>
-      <c r="C34" s="77"/>
+      <c r="C34" s="79"/>
       <c r="D34" s="10"/>
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
@@ -2704,7 +2815,7 @@
     <row r="38" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="16"/>
       <c r="B38" s="6"/>
-      <c r="C38" s="78" t="s">
+      <c r="C38" s="80" t="s">
         <v>15</v>
       </c>
       <c r="D38" s="10"/>
@@ -2725,7 +2836,7 @@
     <row r="39" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="16"/>
       <c r="B39" s="6"/>
-      <c r="C39" s="78"/>
+      <c r="C39" s="80"/>
       <c r="D39" s="10"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
@@ -2763,7 +2874,7 @@
     <row r="41" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="16"/>
       <c r="B41" s="6"/>
-      <c r="C41" s="78" t="s">
+      <c r="C41" s="80" t="s">
         <v>14</v>
       </c>
       <c r="D41" s="10"/>
@@ -2784,7 +2895,7 @@
     <row r="42" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="16"/>
       <c r="B42" s="6"/>
-      <c r="C42" s="78"/>
+      <c r="C42" s="80"/>
       <c r="D42" s="10"/>
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
@@ -2822,7 +2933,7 @@
     <row r="44" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="16"/>
       <c r="B44" s="6"/>
-      <c r="C44" s="78" t="s">
+      <c r="C44" s="80" t="s">
         <v>155</v>
       </c>
       <c r="D44" s="10"/>
@@ -2843,7 +2954,7 @@
     <row r="45" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="16"/>
       <c r="B45" s="6"/>
-      <c r="C45" s="78"/>
+      <c r="C45" s="80"/>
       <c r="D45" s="10"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
@@ -2881,7 +2992,7 @@
     <row r="47" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="16"/>
       <c r="B47" s="6"/>
-      <c r="C47" s="78" t="s">
+      <c r="C47" s="80" t="s">
         <v>132</v>
       </c>
       <c r="D47" s="10"/>
@@ -2902,7 +3013,7 @@
     <row r="48" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="16"/>
       <c r="B48" s="6"/>
-      <c r="C48" s="78"/>
+      <c r="C48" s="80"/>
       <c r="D48" s="10"/>
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
@@ -2940,7 +3051,7 @@
     <row r="50" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="16"/>
       <c r="B50" s="6"/>
-      <c r="C50" s="78" t="s">
+      <c r="C50" s="80" t="s">
         <v>156</v>
       </c>
       <c r="D50" s="10"/>
@@ -2961,7 +3072,7 @@
     <row r="51" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="16"/>
       <c r="B51" s="6"/>
-      <c r="C51" s="78"/>
+      <c r="C51" s="80"/>
       <c r="D51" s="10"/>
       <c r="E51" s="6"/>
       <c r="F51" s="6"/>
@@ -3020,7 +3131,7 @@
     <row r="54" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="16"/>
       <c r="B54" s="6"/>
-      <c r="C54" s="72" t="s">
+      <c r="C54" s="74" t="s">
         <v>133</v>
       </c>
       <c r="D54" s="10"/>
@@ -3041,7 +3152,7 @@
     <row r="55" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="16"/>
       <c r="B55" s="6"/>
-      <c r="C55" s="72"/>
+      <c r="C55" s="74"/>
       <c r="D55" s="10"/>
       <c r="E55" s="6"/>
       <c r="F55" s="6"/>
@@ -3079,7 +3190,7 @@
     <row r="57" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="16"/>
       <c r="B57" s="6"/>
-      <c r="C57" s="72" t="s">
+      <c r="C57" s="74" t="s">
         <v>134</v>
       </c>
       <c r="D57" s="10"/>
@@ -3100,7 +3211,7 @@
     <row r="58" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="16"/>
       <c r="B58" s="6"/>
-      <c r="C58" s="72"/>
+      <c r="C58" s="74"/>
       <c r="D58" s="10"/>
       <c r="E58" s="6"/>
       <c r="F58" s="6"/>
@@ -3138,7 +3249,7 @@
     <row r="60" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="16"/>
       <c r="B60" s="6"/>
-      <c r="C60" s="72" t="s">
+      <c r="C60" s="74" t="s">
         <v>154</v>
       </c>
       <c r="D60" s="10"/>
@@ -3159,7 +3270,7 @@
     <row r="61" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="16"/>
       <c r="B61" s="6"/>
-      <c r="C61" s="72"/>
+      <c r="C61" s="74"/>
       <c r="D61" s="10"/>
       <c r="E61" s="6"/>
       <c r="F61" s="6"/>
@@ -3197,7 +3308,7 @@
     <row r="63" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="16"/>
       <c r="B63" s="6"/>
-      <c r="C63" s="72" t="s">
+      <c r="C63" s="74" t="s">
         <v>153</v>
       </c>
       <c r="D63" s="10"/>
@@ -3218,7 +3329,7 @@
     <row r="64" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="16"/>
       <c r="B64" s="6"/>
-      <c r="C64" s="72"/>
+      <c r="C64" s="74"/>
       <c r="D64" s="10"/>
       <c r="E64" s="6"/>
       <c r="F64" s="6"/>
@@ -3256,7 +3367,7 @@
     <row r="66" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="16"/>
       <c r="B66" s="6"/>
-      <c r="C66" s="72" t="s">
+      <c r="C66" s="74" t="s">
         <v>152</v>
       </c>
       <c r="D66" s="10"/>
@@ -3277,7 +3388,7 @@
     <row r="67" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="16"/>
       <c r="B67" s="6"/>
-      <c r="C67" s="72"/>
+      <c r="C67" s="74"/>
       <c r="D67" s="10"/>
       <c r="E67" s="6"/>
       <c r="F67" s="6"/>
@@ -3315,7 +3426,7 @@
     <row r="69" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="16"/>
       <c r="B69" s="6"/>
-      <c r="C69" s="72" t="s">
+      <c r="C69" s="74" t="s">
         <v>151</v>
       </c>
       <c r="D69" s="10"/>
@@ -3336,7 +3447,7 @@
     <row r="70" spans="1:68" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="16"/>
       <c r="B70" s="6"/>
-      <c r="C70" s="72"/>
+      <c r="C70" s="74"/>
       <c r="D70" s="10"/>
       <c r="E70" s="6"/>
       <c r="F70" s="6"/>
@@ -3374,7 +3485,7 @@
     <row r="72" spans="1:68" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="16"/>
       <c r="B72" s="6"/>
-      <c r="C72" s="73" t="s">
+      <c r="C72" s="75" t="s">
         <v>56</v>
       </c>
       <c r="D72" s="7"/>
@@ -3395,7 +3506,7 @@
     <row r="73" spans="1:68" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="16"/>
       <c r="B73" s="6"/>
-      <c r="C73" s="73"/>
+      <c r="C73" s="75"/>
       <c r="D73" s="7"/>
       <c r="E73" s="6"/>
       <c r="F73" s="6"/>
@@ -3414,7 +3525,7 @@
     <row r="74" spans="1:68" s="5" customFormat="1" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="16"/>
       <c r="B74" s="6"/>
-      <c r="C74" s="75" t="s">
+      <c r="C74" s="77" t="s">
         <v>127</v>
       </c>
       <c r="D74" s="7"/>
@@ -3485,7 +3596,7 @@
     <row r="75" spans="1:68" s="5" customFormat="1" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="16"/>
       <c r="B75" s="6"/>
-      <c r="C75" s="75"/>
+      <c r="C75" s="77"/>
       <c r="D75" s="7"/>
       <c r="E75" s="6"/>
       <c r="F75" s="6"/>
@@ -3613,18 +3724,18 @@
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
       <c r="E79" s="5"/>
-      <c r="F79" s="74"/>
-      <c r="G79" s="74"/>
+      <c r="F79" s="76"/>
+      <c r="G79" s="76"/>
       <c r="H79" s="6"/>
       <c r="I79" s="38" t="s">
         <v>58</v>
       </c>
       <c r="J79" s="38"/>
       <c r="K79" s="6"/>
-      <c r="L79" s="71" t="s">
+      <c r="L79" s="73" t="s">
         <v>57</v>
       </c>
-      <c r="M79" s="71"/>
+      <c r="M79" s="73"/>
       <c r="N79" s="40"/>
       <c r="O79" s="5"/>
       <c r="P79" s="5"/>
@@ -3707,7 +3818,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="87" t="s">
+      <c r="A3" s="89" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -3717,7 +3828,7 @@
       <c r="D3" s="59"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="87"/>
+      <c r="A4" s="89"/>
       <c r="B4" s="1" t="s">
         <v>137</v>
       </c>
@@ -3732,7 +3843,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="87"/>
+      <c r="A5" s="89"/>
       <c r="B5" s="1" t="s">
         <v>138</v>
       </c>
@@ -3792,10 +3903,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C39"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3803,21 +3914,97 @@
     <col min="1" max="1" width="29.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C1" s="108"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>149</v>
       </c>
       <c r="C2" s="61"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>148</v>
       </c>
       <c r="C3" s="60"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C5" s="72"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>198</v>
+      </c>
+      <c r="C6" s="106"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>197</v>
+      </c>
+      <c r="C7" s="107"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>204</v>
+      </c>
+      <c r="C10" s="109"/>
+      <c r="D10" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>200</v>
+      </c>
+      <c r="C11" s="110"/>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>202</v>
+      </c>
+      <c r="C12" s="111"/>
+      <c r="D12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>203</v>
+      </c>
+      <c r="C13" s="107"/>
+      <c r="D13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>201</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -3922,6 +4109,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3968,7 +4156,7 @@
       </c>
     </row>
     <row r="3" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="88" t="s">
+      <c r="B3" s="90" t="s">
         <v>41</v>
       </c>
       <c r="C3" s="44" t="s">
@@ -3987,11 +4175,11 @@
       </c>
     </row>
     <row r="4" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="89"/>
-      <c r="C4" s="92" t="s">
+      <c r="B4" s="91"/>
+      <c r="C4" s="94" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="92" t="s">
+      <c r="D4" s="94" t="s">
         <v>40</v>
       </c>
       <c r="E4" s="45" t="s">
@@ -4004,9 +4192,9 @@
       </c>
     </row>
     <row r="5" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="89"/>
-      <c r="C5" s="89"/>
-      <c r="D5" s="89"/>
+      <c r="B5" s="91"/>
+      <c r="C5" s="91"/>
+      <c r="D5" s="91"/>
       <c r="E5" s="45" t="s">
         <v>162</v>
       </c>
@@ -4021,9 +4209,9 @@
       </c>
     </row>
     <row r="6" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="89"/>
-      <c r="C6" s="89"/>
-      <c r="D6" s="89"/>
+      <c r="B6" s="91"/>
+      <c r="C6" s="91"/>
+      <c r="D6" s="91"/>
       <c r="E6" s="45" t="s">
         <v>163</v>
       </c>
@@ -4038,9 +4226,9 @@
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="90"/>
-      <c r="C7" s="90"/>
-      <c r="D7" s="90"/>
+      <c r="B7" s="92"/>
+      <c r="C7" s="92"/>
+      <c r="D7" s="92"/>
       <c r="E7" s="45" t="s">
         <v>185</v>
       </c>
@@ -4116,13 +4304,13 @@
       <c r="H12" s="45"/>
     </row>
     <row r="13" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="101" t="s">
+      <c r="B13" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="94" t="s">
+      <c r="C13" s="96" t="s">
         <v>70</v>
       </c>
-      <c r="D13" s="94" t="s">
+      <c r="D13" s="96" t="s">
         <v>71</v>
       </c>
       <c r="E13" s="47" t="s">
@@ -4135,9 +4323,9 @@
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B14" s="102"/>
-      <c r="C14" s="95"/>
-      <c r="D14" s="95"/>
+      <c r="B14" s="104"/>
+      <c r="C14" s="97"/>
+      <c r="D14" s="97"/>
       <c r="E14" s="47" t="s">
         <v>72</v>
       </c>
@@ -4152,7 +4340,7 @@
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B15" s="102"/>
+      <c r="B15" s="104"/>
       <c r="C15" s="47" t="s">
         <v>75</v>
       </c>
@@ -4171,11 +4359,11 @@
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="102"/>
-      <c r="C16" s="94" t="s">
+      <c r="B16" s="104"/>
+      <c r="C16" s="96" t="s">
         <v>79</v>
       </c>
-      <c r="D16" s="94" t="s">
+      <c r="D16" s="96" t="s">
         <v>80</v>
       </c>
       <c r="E16" s="47" t="s">
@@ -4188,9 +4376,9 @@
       </c>
     </row>
     <row r="17" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="102"/>
-      <c r="C17" s="95"/>
-      <c r="D17" s="95"/>
+      <c r="B17" s="104"/>
+      <c r="C17" s="97"/>
+      <c r="D17" s="97"/>
       <c r="E17" s="47" t="s">
         <v>82</v>
       </c>
@@ -4205,7 +4393,7 @@
       </c>
     </row>
     <row r="18" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="102"/>
+      <c r="B18" s="104"/>
       <c r="C18" s="66"/>
       <c r="D18" s="66"/>
       <c r="E18" s="48"/>
@@ -4214,7 +4402,7 @@
       <c r="H18" s="48"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="102"/>
+      <c r="B19" s="104"/>
       <c r="C19" s="48" t="s">
         <v>89</v>
       </c>
@@ -4233,47 +4421,47 @@
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="102"/>
+      <c r="B20" s="104"/>
       <c r="C20" s="48"/>
       <c r="D20" s="48"/>
       <c r="E20" s="48"/>
       <c r="F20" s="48"/>
-      <c r="G20" s="104"/>
+      <c r="G20" s="71"/>
       <c r="H20" s="48"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="102"/>
+      <c r="B21" s="104"/>
       <c r="C21" s="48"/>
       <c r="D21" s="48"/>
       <c r="E21" s="48"/>
       <c r="F21" s="48"/>
-      <c r="G21" s="104"/>
+      <c r="G21" s="71"/>
       <c r="H21" s="48"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="102"/>
+      <c r="B22" s="104"/>
       <c r="C22" s="48"/>
       <c r="D22" s="48"/>
       <c r="E22" s="48"/>
       <c r="F22" s="48"/>
-      <c r="G22" s="104"/>
+      <c r="G22" s="71"/>
       <c r="H22" s="48"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="102"/>
+      <c r="B23" s="104"/>
       <c r="C23" s="48"/>
       <c r="D23" s="48"/>
       <c r="E23" s="48"/>
       <c r="F23" s="48"/>
-      <c r="G23" s="104"/>
+      <c r="G23" s="71"/>
       <c r="H23" s="48"/>
     </row>
     <row r="24" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="102"/>
-      <c r="C24" s="91" t="s">
+      <c r="B24" s="104"/>
+      <c r="C24" s="93" t="s">
         <v>43</v>
       </c>
-      <c r="D24" s="91" t="s">
+      <c r="D24" s="93" t="s">
         <v>47</v>
       </c>
       <c r="E24" s="49" t="s">
@@ -4286,9 +4474,9 @@
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="102"/>
-      <c r="C25" s="91"/>
-      <c r="D25" s="91"/>
+      <c r="B25" s="104"/>
+      <c r="C25" s="93"/>
+      <c r="D25" s="93"/>
       <c r="E25" s="49" t="s">
         <v>93</v>
       </c>
@@ -4301,7 +4489,7 @@
       <c r="H25" s="49"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="102"/>
+      <c r="B26" s="104"/>
       <c r="C26" s="49" t="s">
         <v>44</v>
       </c>
@@ -4320,7 +4508,7 @@
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="102"/>
+      <c r="B27" s="104"/>
       <c r="C27" s="49" t="s">
         <v>45</v>
       </c>
@@ -4341,11 +4529,11 @@
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B28" s="102"/>
-      <c r="C28" s="96" t="s">
+      <c r="B28" s="104"/>
+      <c r="C28" s="98" t="s">
         <v>46</v>
       </c>
-      <c r="D28" s="96" t="s">
+      <c r="D28" s="98" t="s">
         <v>54</v>
       </c>
       <c r="E28" s="49" t="s">
@@ -4360,9 +4548,9 @@
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B29" s="102"/>
-      <c r="C29" s="97"/>
-      <c r="D29" s="97"/>
+      <c r="B29" s="104"/>
+      <c r="C29" s="99"/>
+      <c r="D29" s="99"/>
       <c r="E29" s="49" t="s">
         <v>97</v>
       </c>
@@ -4377,7 +4565,7 @@
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B30" s="102"/>
+      <c r="B30" s="104"/>
       <c r="C30" s="49" t="s">
         <v>50</v>
       </c>
@@ -4398,7 +4586,7 @@
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B31" s="102"/>
+      <c r="B31" s="104"/>
       <c r="C31" s="65"/>
       <c r="D31" s="65"/>
       <c r="E31" s="69"/>
@@ -4407,7 +4595,7 @@
       <c r="H31" s="69"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B32" s="102"/>
+      <c r="B32" s="104"/>
       <c r="C32" s="65"/>
       <c r="D32" s="65"/>
       <c r="E32" s="69"/>
@@ -4416,7 +4604,7 @@
       <c r="H32" s="69"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B33" s="102"/>
+      <c r="B33" s="104"/>
       <c r="C33" s="65"/>
       <c r="D33" s="65"/>
       <c r="E33" s="69"/>
@@ -4425,7 +4613,7 @@
       <c r="H33" s="69"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B34" s="102"/>
+      <c r="B34" s="104"/>
       <c r="C34" s="65"/>
       <c r="D34" s="65"/>
       <c r="E34" s="69"/>
@@ -4434,7 +4622,7 @@
       <c r="H34" s="69"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B35" s="102"/>
+      <c r="B35" s="104"/>
       <c r="C35" s="65"/>
       <c r="D35" s="65"/>
       <c r="E35" s="69"/>
@@ -4443,7 +4631,7 @@
       <c r="H35" s="69"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B36" s="102"/>
+      <c r="B36" s="104"/>
       <c r="C36" s="65"/>
       <c r="D36" s="65"/>
       <c r="E36" s="69"/>
@@ -4452,11 +4640,11 @@
       <c r="H36" s="69"/>
     </row>
     <row r="37" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="102"/>
-      <c r="C37" s="96" t="s">
+      <c r="B37" s="104"/>
+      <c r="C37" s="98" t="s">
         <v>51</v>
       </c>
-      <c r="D37" s="96" t="s">
+      <c r="D37" s="98" t="s">
         <v>52</v>
       </c>
       <c r="E37" s="49" t="s">
@@ -4473,9 +4661,9 @@
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B38" s="103"/>
-      <c r="C38" s="97"/>
-      <c r="D38" s="97"/>
+      <c r="B38" s="105"/>
+      <c r="C38" s="99"/>
+      <c r="D38" s="99"/>
       <c r="E38" s="49" t="s">
         <v>100</v>
       </c>
@@ -4490,13 +4678,13 @@
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B39" s="98" t="s">
+      <c r="B39" s="100" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="93" t="s">
+      <c r="C39" s="95" t="s">
         <v>59</v>
       </c>
-      <c r="D39" s="93" t="s">
+      <c r="D39" s="95" t="s">
         <v>61</v>
       </c>
       <c r="E39" s="46" t="s">
@@ -4509,9 +4697,9 @@
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B40" s="99"/>
-      <c r="C40" s="93"/>
-      <c r="D40" s="93"/>
+      <c r="B40" s="101"/>
+      <c r="C40" s="95"/>
+      <c r="D40" s="95"/>
       <c r="E40" s="46" t="s">
         <v>60</v>
       </c>
@@ -4526,7 +4714,7 @@
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B41" s="99"/>
+      <c r="B41" s="101"/>
       <c r="C41" s="63"/>
       <c r="D41" s="63"/>
       <c r="E41" s="63"/>
@@ -4535,7 +4723,7 @@
       <c r="H41" s="63"/>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B42" s="100"/>
+      <c r="B42" s="102"/>
       <c r="C42" s="46" t="s">
         <v>62</v>
       </c>
@@ -4621,13 +4809,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="B39:B42"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="B13:B38"/>
     <mergeCell ref="C28:C29"/>
     <mergeCell ref="B3:B7"/>
     <mergeCell ref="C24:C25"/>
@@ -4638,6 +4819,13 @@
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="D13:D14"/>
     <mergeCell ref="D24:D25"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="B13:B38"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>